<commit_message>
Update backend and frontend files
</commit_message>
<xml_diff>
--- a/backend/submissions.xlsx
+++ b/backend/submissions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,33 @@
   </si>
   <si>
     <t>nd ,</t>
+  </si>
+  <si>
+    <t>vb v n j</t>
+  </si>
+  <si>
+    <t>Mehak yadav</t>
+  </si>
+  <si>
+    <t>NSUT</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  b  u  u</t>
+  </si>
+  <si>
+    <t>Mehak</t>
+  </si>
+  <si>
+    <t>6000000</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>knejivie</t>
   </si>
 </sst>
 </file>
@@ -423,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -466,8 +493,188 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>